<commit_message>
Export excel for grafic, improvment user, add regionId
</commit_message>
<xml_diff>
--- a/src/main/resources/testFile2.xlsx
+++ b/src/main/resources/testFile2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>Ð/Ð</t>
   </si>
@@ -139,6 +139,48 @@
   </si>
   <si>
     <t>ë -1      ÷-1</t>
+  </si>
+  <si>
+    <t>000008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Մնացականյան Էդուարդ </t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>eewr,werwer,</t>
+  </si>
+  <si>
+    <t>000007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Սահակյան Վալերի </t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>sdfsd,dsfdsf,sd,111,</t>
+  </si>
+  <si>
+    <t>000006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Հակոբյան Արթուր </t>
+  </si>
+  <si>
+    <t>000009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Մանուչարյան Կամո </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sas, sadsa, 12, </t>
   </si>
   <si>
     <t>Updated Value</t>
@@ -815,46 +857,58 @@
       <c r="A6" s="8">
         <v>1</v>
       </c>
-      <c r="B6" s="3">
-        <v>115362</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>12.0</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="19">
-        <v>273018</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E6" s="19"/>
       <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19">
-        <v>1</v>
-      </c>
-      <c r="I6" s="19"/>
+      <c r="G6" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>43</v>
+      </c>
       <c r="J6" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>43</v>
       </c>
       <c r="P6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="Q6" s="22">
-        <v>43025</v>
-      </c>
-      <c r="R6" s="19"/>
+      <c r="Q6" s="22" t="n">
+        <v>42640.0</v>
+      </c>
+      <c r="R6" s="19" t="n">
+        <v>42823.0</v>
+      </c>
       <c r="S6" s="4">
         <v>16</v>
       </c>
       <c r="T6" s="21" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="U6" s="19"/>
       <c r="V6" s="19"/>
@@ -862,7 +916,7 @@
     <row customHeight="1" ht="15.95" r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>34</v>
@@ -891,31 +945,57 @@
       <c r="A8" s="8">
         <v>2</v>
       </c>
-      <c r="B8" s="3">
-        <v>114414</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="17"/>
+      <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
+      <c r="G8" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>43</v>
+      </c>
       <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
+      <c r="Q8" s="19" t="n">
+        <v>42640.0</v>
+      </c>
+      <c r="R8" s="19" t="n">
+        <v>42823.0</v>
+      </c>
       <c r="S8" s="4">
         <v>16</v>
       </c>
-      <c r="T8" s="19"/>
+      <c r="T8" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="U8" s="19"/>
       <c r="V8" s="19"/>
     </row>
@@ -947,25 +1027,51 @@
       <c r="A10" s="8">
         <v>3</v>
       </c>
-      <c r="B10" s="3">
-        <v>114415</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="17"/>
+      <c r="B10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>51</v>
+      </c>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
+      <c r="G10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="O10" s="19" t="s">
+        <v>43</v>
+      </c>
       <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
+      <c r="Q10" s="19" t="n">
+        <v>42640.0</v>
+      </c>
+      <c r="R10" s="19" t="n">
+        <v>42823.0</v>
+      </c>
       <c r="S10" s="2"/>
       <c r="T10" s="19"/>
       <c r="U10" s="19"/>
@@ -999,27 +1105,55 @@
       <c r="A12" s="8">
         <v>4</v>
       </c>
-      <c r="B12" s="3">
-        <v>114111</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="17"/>
+      <c r="B12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
+      <c r="G12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>43</v>
+      </c>
       <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
+      <c r="Q12" s="19" t="n">
+        <v>42402.0</v>
+      </c>
+      <c r="R12" s="19" t="n">
+        <v>42585.0</v>
+      </c>
       <c r="S12" s="2"/>
-      <c r="T12" s="19"/>
+      <c r="T12" s="19" t="s">
+        <v>54</v>
+      </c>
       <c r="U12" s="19"/>
       <c r="V12" s="19"/>
     </row>

</xml_diff>